<commit_message>
Add Order ID to excel
</commit_message>
<xml_diff>
--- a/NANO_KAFFEE_GmbH_YYYY_MM_Abt.3A.xlsx
+++ b/NANO_KAFFEE_GmbH_YYYY_MM_Abt.3A.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">NANO KAFFEE GmbH </t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ausgangsbestätigung / Ausgangsvermerk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OrderID</t>
   </si>
 </sst>
 </file>
@@ -278,79 +281,79 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -606,8 +609,8 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R16" activeCellId="0" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1192,7 +1195,9 @@
       <c r="Q14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="R14" s="7"/>
+      <c r="R14" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>

</xml_diff>

<commit_message>
Fix equation in A3-template
</commit_message>
<xml_diff>
--- a/NANO_KAFFEE_GmbH_YYYY_MM_Abt.3A.xlsx
+++ b/NANO_KAFFEE_GmbH_YYYY_MM_Abt.3A.xlsx
@@ -609,8 +609,8 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R16" activeCellId="0" sqref="R16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -953,7 +953,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="n">
-        <v>75.74</v>
+        <v>0</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="2"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="C11" s="13" t="n">
         <f aca="false">C9+C10</f>
-        <v>75.74</v>
+        <v>0</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="2"/>

</xml_diff>